<commit_message>
get users by weight
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -434,7 +434,8 @@
     <col width="30" customWidth="1" min="1" max="1"/>
     <col width="20" customWidth="1" min="2" max="2"/>
     <col width="10" customWidth="1" min="3" max="3"/>
-    <col width="25" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="4" max="4"/>
+    <col width="25" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -455,10 +456,14 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Referallar soni</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>Ro'xatdan o'tgan vaqti</t>
         </is>
       </c>
-      <c r="E1" s="2" t="n"/>
       <c r="F1" s="2" t="n"/>
       <c r="G1" s="2" t="n"/>
       <c r="H1" s="2" t="n"/>
@@ -467,7 +472,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>Sanjarbek</t>
+          <t>sa</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
@@ -476,11 +481,14 @@
         </is>
       </c>
       <c r="C2" s="3" t="n">
-        <v>77</v>
-      </c>
-      <c r="D2" s="3" t="inlineStr">
-        <is>
-          <t>2023-11-23 04:45:41</t>
+        <v>33</v>
+      </c>
+      <c r="D2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3" t="inlineStr">
+        <is>
+          <t>2023-11-23 07:46:17</t>
         </is>
       </c>
     </row>

</xml_diff>